<commit_message>
Data display and internal review files
Pull everything together for data display and internal review
</commit_message>
<xml_diff>
--- a/Other tools/Standard_layer_display/BenUse_standards_relation_tables.xlsx
+++ b/Other tools/Standard_layer_display/BenUse_standards_relation_tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\IR2018\Other tools\Standard_layer_display\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\Users\jmccona\Standards Layers\Beneficial Use Mapping\Beneficial Use Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8505" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="BenUse_codes" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Spawning_dates" sheetId="7" r:id="rId6"/>
     <sheet name="DO_criteria" sheetId="8" r:id="rId7"/>
     <sheet name="pH_criteria" sheetId="9" r:id="rId8"/>
-    <sheet name="ALtoxics_criteria" sheetId="10" r:id="rId9"/>
+    <sheet name="Bacteria_criteria" sheetId="11" r:id="rId9"/>
+    <sheet name="ALtoxics_criteria" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BenUse_codes!$A$1:$A$21</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="174">
   <si>
     <t>ben_use_code</t>
   </si>
@@ -548,6 +549,33 @@
   </si>
   <si>
     <t>WDMC Site specific criteria</t>
+  </si>
+  <si>
+    <t>bacteria_criteria</t>
+  </si>
+  <si>
+    <t>bacteria_code</t>
+  </si>
+  <si>
+    <t>Coastal Contact Recreation</t>
+  </si>
+  <si>
+    <t>Freshwater Contact Recreation</t>
+  </si>
+  <si>
+    <t>Coastal Contact Recreation and Fishing - Shellfish Harvesting</t>
+  </si>
+  <si>
+    <t>bacteria_indicator</t>
+  </si>
+  <si>
+    <t>E. coli</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>Enterococcus &amp; Fecal Coliform</t>
   </si>
 </sst>
 </file>
@@ -915,7 +943,7 @@
   <dimension ref="A1:C150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A2" sqref="A2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,12 +2617,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B19" sqref="B19:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,7 +2953,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,7 +3847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="A205" sqref="A205:XFD209"/>
     </sheetView>
   </sheetViews>
@@ -7553,8 +7646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7882,7 +7975,7 @@
   <dimension ref="A16:B23"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7965,7 +8058,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8054,62 +8147,89 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="5">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>